<commit_message>
upload new part 2 and test macro workbooks
</commit_message>
<xml_diff>
--- a/images/IntroExcel-Part2-SampleWorkbook.xlsx
+++ b/images/IntroExcel-Part2-SampleWorkbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\UI Library\Liaison Work\Library Instruction\Library Workshops\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\UI Library\Liaison Work\Library Instruction\Library Workshops\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="102">
   <si>
     <t>Student</t>
   </si>
@@ -108,9 +109,6 @@
     <t>state</t>
   </si>
   <si>
-    <t>Saleperson</t>
-  </si>
-  <si>
     <t>Sales Q1</t>
   </si>
   <si>
@@ -127,6 +125,213 @@
   </si>
   <si>
     <t>delaware</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Title_Remark</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Pub_Year</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>Binding</t>
+  </si>
+  <si>
+    <t>COLLECTIVE MEMORY WORK: A METHODOLOGY FOR LEARNING WITH AND FROM LIVED EXPERIENCE</t>
+  </si>
+  <si>
+    <t>ROUTLEDGE</t>
+  </si>
+  <si>
+    <t>eBook</t>
+  </si>
+  <si>
+    <t>COMPASSIONATE MIGRATION AND REGIONAL POLICY IN THE AMERICAS</t>
+  </si>
+  <si>
+    <t>PALGRAVE MACMILLAN</t>
+  </si>
+  <si>
+    <t>GENDERING NATIONALISM: INTERSECTIONS OF NATION, GENDER AND SEXUALITY</t>
+  </si>
+  <si>
+    <t>GRIDDED WORLDS: AN URBAN ANTHOLOGY</t>
+  </si>
+  <si>
+    <t>SPRINGER</t>
+  </si>
+  <si>
+    <t>HANDBOOK OF COMMUNITY MOVEMENTS AND LOCAL ORGANIZATIONS IN THE 21ST CENTURY</t>
+  </si>
+  <si>
+    <t>IMAGE POLITICS OF CLIMATE CHANGE: VISUALIZATIONS, IMAGINATIONS, DOCUMENTATIONS</t>
+  </si>
+  <si>
+    <t>TRANSCRIPT</t>
+  </si>
+  <si>
+    <t>IMMIGRATION AND METROPOLITAN REVITALIZATION IN THE UNITED ST.</t>
+  </si>
+  <si>
+    <t>DOMENIC VITIELLO</t>
+  </si>
+  <si>
+    <t>UNIV PENN PRESS</t>
+  </si>
+  <si>
+    <t>IMMIGRATION POLICY IN THE AGE OF PUNISHMENT: DETENTION, DEPORTATION, AND BORDER CONTROL.</t>
+  </si>
+  <si>
+    <t>COLUMBIA UNIVERSITY PRESS</t>
+  </si>
+  <si>
+    <t>LAND RIGHTS, BIODIVERSITY CONSERVATION AND JUSTICE: RETHINKING PARKS AND PEOPLE</t>
+  </si>
+  <si>
+    <t>MACHINE LEARNING TECHNIQUES FOR ONLINE SOCIAL NETWORKS</t>
+  </si>
+  <si>
+    <t>MODERN AMERICAN EXTREMISM AND DOMESTIC TERRORISM: AN ENCYCLOPEDIA OF EXTREMISTS AND EXTREMIST GROUPS.</t>
+  </si>
+  <si>
+    <t>ABC-CLIO</t>
+  </si>
+  <si>
+    <t>ON REPLACEMENT: CULTURAL, SOCIAL AND PSYCHOLOGICAL REPRESENTATIONS</t>
+  </si>
+  <si>
+    <t>ORGANIZING NETWORKS: AN ACTOR-NETWORK THEORY OF ORGANIZATIONS.</t>
+  </si>
+  <si>
+    <t>POLITICS, POWER AND COMMUNITY DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>POLICY PRESS</t>
+  </si>
+  <si>
+    <t>REVEALING TACIT KNOWLEDGE: EMBODIMENT AND EXPLICATION</t>
+  </si>
+  <si>
+    <t>TRANSCRIPT VERLAG</t>
+  </si>
+  <si>
+    <t>RURAL POVERTY IN THE UNITED STATES</t>
+  </si>
+  <si>
+    <t>SHARED PROSPERITY IN AMERICA'S COMMUNITIES</t>
+  </si>
+  <si>
+    <t>UNIV OF PENNSYLVANIA PR</t>
+  </si>
+  <si>
+    <t>SOCIAL THEORIES OF URBAN VIOLENCE IN THE GLOBAL SOUTH: TOWARDS SAFE AND INCLUSIVE CITIES</t>
+  </si>
+  <si>
+    <t>THICK SPACE.</t>
+  </si>
+  <si>
+    <t>TRANSCRIPT-VERLAG</t>
+  </si>
+  <si>
+    <t>URBAN TRANSFORMATIONS IN THE U.S.A.: SPACES, COMMUNITIES, REPRESENTATIONS</t>
+  </si>
+  <si>
+    <t>WHAT IS A SLAVE SOCIETY?: THE PRACTICE OF SLAVERY IN GLOBAL PERSPECTIVE</t>
+  </si>
+  <si>
+    <t>CAMBRIDGE UNIV PRESS</t>
+  </si>
+  <si>
+    <t>WILDLIFE CRIME: FROM THEORY TO PRACTICE</t>
+  </si>
+  <si>
+    <t>TEMPLE UNIVERSITY PRESS</t>
+  </si>
+  <si>
+    <t>WORLDWIDE MOBILIZATIONS: CLASS STRUGGLES AND URBAN COMMONING</t>
+  </si>
+  <si>
+    <t>BERGHAHN BOOKS</t>
+  </si>
+  <si>
+    <t>COREY W. JOHNSON</t>
+  </si>
+  <si>
+    <t>STEVEN W. BENDER</t>
+  </si>
+  <si>
+    <t>JON MULHOLLAND</t>
+  </si>
+  <si>
+    <t>REUBEN ROSE-REDWOOD</t>
+  </si>
+  <si>
+    <t>RAM A. CNAAN</t>
+  </si>
+  <si>
+    <t>BIRGIT SCHNEIDER</t>
+  </si>
+  <si>
+    <t>DAVID C. BROTHERTON</t>
+  </si>
+  <si>
+    <t>SHARLENE MOLLETT</t>
+  </si>
+  <si>
+    <t>TANSEL OZYER</t>
+  </si>
+  <si>
+    <t>BARRY J. BALLECK</t>
+  </si>
+  <si>
+    <t>JEAN OWEN</t>
+  </si>
+  <si>
+    <t>ANDREA BELLINGER</t>
+  </si>
+  <si>
+    <t>ROSIE MEADE</t>
+  </si>
+  <si>
+    <t>FRANK ADLOFF</t>
+  </si>
+  <si>
+    <t>ANN R. TICKAMYER</t>
+  </si>
+  <si>
+    <t>SUSAN M. WACHTER</t>
+  </si>
+  <si>
+    <t>JENNIFER ERIN SALAHUB</t>
+  </si>
+  <si>
+    <t>DOROTHEE BRANTZ</t>
+  </si>
+  <si>
+    <t>JULIA SATTLER</t>
+  </si>
+  <si>
+    <t>NOEL LENSKI</t>
+  </si>
+  <si>
+    <t>WILLIAM D. MORETO</t>
+  </si>
+  <si>
+    <t>DON KALB</t>
+  </si>
+  <si>
+    <t>Salesperson</t>
   </si>
 </sst>
 </file>
@@ -450,7 +655,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,24 +668,24 @@
         <v>26</v>
       </c>
       <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -502,7 +707,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -523,7 +728,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -544,7 +749,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -565,7 +770,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -586,7 +791,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -607,7 +812,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -628,7 +833,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -649,7 +854,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -670,7 +875,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -691,7 +896,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -712,7 +917,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -733,7 +938,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -754,7 +959,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -775,7 +980,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -796,7 +1001,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -817,7 +1022,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -838,7 +1043,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -859,7 +1064,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -880,7 +1085,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -901,7 +1106,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -922,7 +1127,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1302,4 +1507,503 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2">
+        <v>2018</v>
+      </c>
+      <c r="F2">
+        <v>9781315298696</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>2017</v>
+      </c>
+      <c r="F3">
+        <v>9781137550743</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4">
+        <v>2018</v>
+      </c>
+      <c r="F4">
+        <v>9783319766997</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5">
+        <v>2018</v>
+      </c>
+      <c r="F5">
+        <v>9783319764900</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>2018</v>
+      </c>
+      <c r="F6">
+        <v>9783319774169</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>2014</v>
+      </c>
+      <c r="F7">
+        <v>9783839426104</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8">
+        <v>2017</v>
+      </c>
+      <c r="F8">
+        <v>9780812293951</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9">
+        <v>2018</v>
+      </c>
+      <c r="F9">
+        <v>9780231545891</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10">
+        <v>2018</v>
+      </c>
+      <c r="F10">
+        <v>9781315439464</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11">
+        <v>9783319899329</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12">
+        <v>9781440852756</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13">
+        <v>9783319760117</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>2016</v>
+      </c>
+      <c r="F14">
+        <v>9783839436165</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15">
+        <v>2016</v>
+      </c>
+      <c r="F15">
+        <v>9781447317388</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16">
+        <v>2015</v>
+      </c>
+      <c r="F16">
+        <v>9783839425169</v>
+      </c>
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17">
+        <v>2017</v>
+      </c>
+      <c r="F17">
+        <v>9780231544719</v>
+      </c>
+      <c r="G17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18">
+        <v>2016</v>
+      </c>
+      <c r="F18">
+        <v>9780812292404</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19">
+        <v>2018</v>
+      </c>
+      <c r="F19">
+        <v>9781351254700</v>
+      </c>
+      <c r="G19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20">
+        <v>2014</v>
+      </c>
+      <c r="F20">
+        <v>9783839420430</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21">
+        <v>2016</v>
+      </c>
+      <c r="F21">
+        <v>9783839431115</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22">
+        <v>2018</v>
+      </c>
+      <c r="F22">
+        <v>9781108633208</v>
+      </c>
+      <c r="G22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23">
+        <v>2018</v>
+      </c>
+      <c r="F23">
+        <v>9781439914731</v>
+      </c>
+      <c r="G23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24">
+        <v>2018</v>
+      </c>
+      <c r="F24">
+        <v>9781785339073</v>
+      </c>
+      <c r="G24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upload new version of excel workbook
</commit_message>
<xml_diff>
--- a/images/IntroExcel-Part2-SampleWorkbook.xlsx
+++ b/images/IntroExcel-Part2-SampleWorkbook.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="124">
   <si>
     <t>Student</t>
   </si>
@@ -332,6 +332,72 @@
   </si>
   <si>
     <t>Salesperson</t>
+  </si>
+  <si>
+    <t>Byers, Jordan</t>
+  </si>
+  <si>
+    <t>Collins, Casey</t>
+  </si>
+  <si>
+    <t>Gellers, Alex</t>
+  </si>
+  <si>
+    <t>Jones, Morgan</t>
+  </si>
+  <si>
+    <t>Lowe, Taylor</t>
+  </si>
+  <si>
+    <t>Quinn, Sam</t>
+  </si>
+  <si>
+    <t>Smith, Riley</t>
+  </si>
+  <si>
+    <t>Thomas, Blake</t>
+  </si>
+  <si>
+    <t>Reynolds, Dylan</t>
+  </si>
+  <si>
+    <t>Smith, James</t>
+  </si>
+  <si>
+    <t>Owen, Michelle</t>
+  </si>
+  <si>
+    <t>Ortega, Raul</t>
+  </si>
+  <si>
+    <t>Chen, Maria</t>
+  </si>
+  <si>
+    <t>Olsen, Leslie</t>
+  </si>
+  <si>
+    <t>Nelson, Jamika</t>
+  </si>
+  <si>
+    <t>Williams, Desmond</t>
+  </si>
+  <si>
+    <t>Cooley, Renee</t>
+  </si>
+  <si>
+    <t>Johnson, Tim</t>
+  </si>
+  <si>
+    <t>Huen, James</t>
+  </si>
+  <si>
+    <t>Ryeo, Annie</t>
+  </si>
+  <si>
+    <t>Morgan, Emma</t>
+  </si>
+  <si>
+    <t>Jones, Jackson</t>
   </si>
 </sst>
 </file>
@@ -654,12 +720,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -688,7 +753,7 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="C2">
         <v>850</v>
@@ -710,7 +775,7 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C3">
         <v>950</v>
@@ -731,7 +796,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="C4">
         <v>300</v>
@@ -752,7 +817,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="C5">
         <v>400</v>
@@ -773,7 +838,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C6">
         <v>1000</v>
@@ -794,7 +859,7 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="C7">
         <v>1200</v>
@@ -815,7 +880,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="C8">
         <v>250</v>
@@ -836,7 +901,7 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>325</v>
@@ -857,7 +922,7 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="C10">
         <v>1000</v>
@@ -878,7 +943,7 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="C11">
         <v>600</v>
@@ -899,7 +964,7 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="C12">
         <v>1150</v>
@@ -920,7 +985,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="C13">
         <v>900</v>
@@ -941,7 +1006,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="C14">
         <v>875</v>
@@ -962,7 +1027,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="C15">
         <v>1000</v>
@@ -983,7 +1048,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="C16">
         <v>1300</v>
@@ -1004,7 +1069,7 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="C17">
         <v>1250</v>
@@ -1025,7 +1090,7 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="C18">
         <v>545</v>
@@ -1046,7 +1111,7 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="C19">
         <v>750</v>
@@ -1067,7 +1132,7 @@
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="C20">
         <v>1000</v>
@@ -1088,7 +1153,7 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="C21">
         <v>800</v>
@@ -1109,7 +1174,7 @@
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>122</v>
       </c>
       <c r="C22">
         <v>700</v>
@@ -1130,7 +1195,7 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="C23">
         <v>450</v>

</xml_diff>